<commit_message>
All the code for the Hotend Test Jig!
Updated BOM
All the code, untested yet
Updated crystal frequency
</commit_message>
<xml_diff>
--- a/BOM/BOM.xlsx
+++ b/BOM/BOM.xlsx
@@ -12,6 +12,7 @@
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$AA$1</definedName>
     <definedName name="testbench_1" localSheetId="0">Hoja1!$A$1:$L$23</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
@@ -146,9 +147,6 @@
     <t>CR0805-JW-102ELF</t>
   </si>
   <si>
-    <t>20MHz</t>
-  </si>
-  <si>
     <t>CRYSTALHC49US</t>
   </si>
   <si>
@@ -417,13 +415,16 @@
   </si>
   <si>
     <t>SMT 6mm switch, EVQQ2 series</t>
+  </si>
+  <si>
+    <t>16MHz</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -439,13 +440,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -457,10 +470,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -468,8 +482,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Buena" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -776,7 +794,7 @@
   <dimension ref="A1:L23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E40" sqref="E39:E40"/>
+      <selection activeCell="A22" sqref="A22:XFD22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -849,633 +867,638 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
+    <row r="2" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
+        <v>2</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="I2" s="3">
+        <v>317500</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <v>6</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="I3" s="3">
+        <v>1551903</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>6</v>
+      </c>
+      <c r="B4" s="3">
+        <v>100</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I4" s="3">
+        <v>1577644</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <v>1</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="I5" s="3">
+        <v>1657934</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <v>20</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D6" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="F2" s="1" t="s">
+      <c r="E6" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="F6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G6" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H6" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="1">
+      <c r="I6" s="3">
         <v>1716765</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
+    <row r="7" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <v>16</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I7" s="3">
+        <v>1740681</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <v>1</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="I8" s="3">
+        <v>1829472</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
+        <v>1</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="I9" s="3">
+        <v>1842224</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
+        <v>7</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="I10" s="3">
+        <v>1843670</v>
+      </c>
+      <c r="K10" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
+        <v>1</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="I11" s="3">
+        <v>1972086</v>
+      </c>
+      <c r="K11" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="L11" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="3">
+        <v>1</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I12" s="3">
+        <v>2008389</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="3">
+        <v>1</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="I13" s="3">
+        <v>2102585</v>
+      </c>
+      <c r="K13" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="L13" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="3">
         <v>6</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>6</v>
-      </c>
-      <c r="B4" s="1">
-        <v>100</v>
-      </c>
-      <c r="C4" s="1" t="s">
+      <c r="B14" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D14" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E14" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="F14" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="G14" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="I14" s="3">
+        <v>2118118</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="3">
+        <v>2</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="I15" s="3">
+        <v>2436975</v>
+      </c>
+      <c r="K15" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="3">
+        <v>7</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="I16" s="3">
+        <v>2447693</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="3">
+        <v>7</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="I17" s="3">
+        <v>2469474</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="3">
+        <v>1</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="G18" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="G4" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I4" s="1">
-        <v>1577644</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>16</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I5" s="1">
-        <v>1740681</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>7</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="I6" s="1">
-        <v>2469474</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
+      <c r="H18" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="I18" s="3">
+        <v>9962913</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="3">
         <v>1</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="I7" s="1">
-        <v>2008389</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>1</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="I8" s="1">
-        <v>1842224</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>2</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="I9" s="1">
-        <v>317500</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>1</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="I10" s="1">
-        <v>1657934</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
-        <v>6</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="I11" s="1">
-        <v>2118118</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
-        <v>7</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="I12" s="1">
-        <v>2447693</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
-        <v>2</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="I13" s="1">
-        <v>2436975</v>
-      </c>
-      <c r="K13" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
-        <v>1</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="I14" s="1">
-        <v>1972086</v>
-      </c>
-      <c r="K14" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="L14" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
-        <v>1</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
-        <v>3</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="I16" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="J16" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
-        <v>1</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="I17" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" s="1">
-        <v>1</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="I18" s="1">
-        <v>2102585</v>
-      </c>
-      <c r="K18" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="L18" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
-        <v>7</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="I19" s="1">
-        <v>1843670</v>
-      </c>
-      <c r="K19" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B19" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="H19" s="3">
+        <v>39303045</v>
+      </c>
+      <c r="I19" s="3">
+        <v>9963553</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>6</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>76</v>
-      </c>
       <c r="C20" s="1" t="s">
-        <v>76</v>
+        <v>17</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>77</v>
+        <v>18</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>118</v>
+        <v>92</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="H20" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="I20" s="1">
-        <v>1551903</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>1</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>121</v>
+        <v>58</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>79</v>
+        <v>58</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>80</v>
+        <v>59</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>81</v>
+        <v>60</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="H21" s="1">
-        <v>39303045</v>
-      </c>
-      <c r="I21" s="1">
-        <v>9963553</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22" s="1">
-        <v>1</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="I22" s="1">
-        <v>1829472</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="3">
+        <v>3</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="I22" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J22" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>1</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>88</v>
+        <v>62</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>88</v>
+        <v>62</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>89</v>
+        <v>63</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>90</v>
+        <v>64</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="I23" s="1">
-        <v>9962913</v>
+        <v>111</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:AA1">
+    <sortState ref="A2:AA23">
+      <sortCondition ref="I1"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>